<commit_message>
exam a first attempt
</commit_message>
<xml_diff>
--- a/ProfessorMesser/PracticeExams.xlsx
+++ b/ProfessorMesser/PracticeExams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\ProfessorMesser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A935AF6-B275-4FD2-831B-7BCF87A5F014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5DBF16-C00C-496E-8BD5-65CC1725BCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
   </bookViews>
   <sheets>
     <sheet name="Exam A" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,128 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>AEG</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>Vishing</t>
+  </si>
+  <si>
+    <t>Spoofing</t>
+  </si>
+  <si>
+    <t>On-Path</t>
+  </si>
+  <si>
+    <t>DDoS</t>
+  </si>
+  <si>
+    <t>Hoax</t>
+  </si>
+  <si>
+    <t>Biometric Reader</t>
+  </si>
+  <si>
+    <t>Environmental Sensors</t>
+  </si>
+  <si>
+    <t>Video Surveillance</t>
+  </si>
+  <si>
+    <t>Smart Card</t>
+  </si>
+  <si>
+    <t>Full-Disk Encription</t>
+  </si>
+  <si>
+    <t>Locking Cabinets</t>
+  </si>
+  <si>
+    <t>Cable Lock</t>
+  </si>
+  <si>
+    <t>HTTPS</t>
+  </si>
+  <si>
+    <t>NTP</t>
+  </si>
+  <si>
+    <t>SRTP</t>
+  </si>
+  <si>
+    <t>SNMPv3</t>
+  </si>
+  <si>
+    <t>SSH</t>
+  </si>
+  <si>
+    <t>Something you have</t>
+  </si>
+  <si>
+    <t>Something you know</t>
+  </si>
+  <si>
+    <t>Something you can do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Something you are </t>
+  </si>
+  <si>
+    <t>Somewhere you are</t>
+  </si>
+  <si>
+    <t>10.2.1.33 10.1.1.7 HTTPS 443 ALLOW</t>
+  </si>
+  <si>
+    <t>10.2.1.47 10.1.1.3 SSH 22 ALLOW</t>
+  </si>
+  <si>
+    <t>10.1.1.2 10.2.1.20 LDAP 3389 ALLOW</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,12 +504,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230E91FC-5241-4086-9BBB-BCECEDDE28FB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
practice exam A attempt 2
</commit_message>
<xml_diff>
--- a/ProfessorMesser/PracticeExams.xlsx
+++ b/ProfessorMesser/PracticeExams.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\ProfessorMesser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2120627-4A3E-4C0C-992A-02EC567B1567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBFDB01-51A5-4369-94EC-00018EE431EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22150" yWindow="3670" windowWidth="21480" windowHeight="11070" activeTab="3" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
   </bookViews>
   <sheets>
     <sheet name="Exam A" sheetId="1" r:id="rId1"/>
     <sheet name="Exam A Answers" sheetId="2" r:id="rId2"/>
     <sheet name="Exam B" sheetId="3" r:id="rId3"/>
     <sheet name="Exam C" sheetId="4" r:id="rId4"/>
+    <sheet name="Exam A 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="108">
   <si>
     <t>B</t>
   </si>
@@ -327,6 +328,42 @@
   </si>
   <si>
     <t>82/90</t>
+  </si>
+  <si>
+    <t>On-path</t>
+  </si>
+  <si>
+    <t>Locking cabinets</t>
+  </si>
+  <si>
+    <t>Video surveillance</t>
+  </si>
+  <si>
+    <t>Full-disk encryption</t>
+  </si>
+  <si>
+    <t>Biometric reader</t>
+  </si>
+  <si>
+    <t>Smart card</t>
+  </si>
+  <si>
+    <t>Cable lock</t>
+  </si>
+  <si>
+    <t>Something you are</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somewhere you are </t>
+  </si>
+  <si>
+    <t>10.1.1.2 10.2.1.20 TCP 389 ALLOW</t>
+  </si>
+  <si>
+    <t>10.2.1.33 10.1.1.7 TCP 443 ALLOW</t>
+  </si>
+  <si>
+    <t>10.2.1.47 10.1.1.3 TCP 22 ALLOW</t>
   </si>
 </sst>
 </file>
@@ -3409,7 +3446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317E6091-B1A7-4EC6-BBEF-8976F22357A5}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
@@ -4538,4 +4575,529 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4841A40-96C6-4B3A-A578-4832E7D72006}">
+  <dimension ref="A1:L90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
exam A attempt 2 answers
</commit_message>
<xml_diff>
--- a/ProfessorMesser/PracticeExams.xlsx
+++ b/ProfessorMesser/PracticeExams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\ProfessorMesser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBFDB01-51A5-4369-94EC-00018EE431EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F22198-BD24-4015-8757-A07E2779FCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="110">
   <si>
     <t>B</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>10.2.1.47 10.1.1.3 TCP 22 ALLOW</t>
+  </si>
+  <si>
+    <t>84/85</t>
+  </si>
+  <si>
+    <t>89/90</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1240,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4581,8 +4587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4841A40-96C6-4B3A-A578-4832E7D72006}">
   <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4670,6 +4676,13 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF(A6=B6, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
       <c r="E6" t="s">
         <v>101</v>
       </c>
@@ -4678,6 +4691,13 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ref="C7:C70" si="0">IF(A7=B7, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
       <c r="E7" t="s">
         <v>102</v>
       </c>
@@ -4685,416 +4705,1003 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" ref="C71:C90" si="1">IF(A71=B71, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>5</v>
+      </c>
+      <c r="B90" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exam b attempt 2
</commit_message>
<xml_diff>
--- a/ProfessorMesser/PracticeExams.xlsx
+++ b/ProfessorMesser/PracticeExams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\ProfessorMesser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4275E7-6C2A-41A5-A468-A00EFC7D3601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2734900E-9F87-4DA0-8DC6-DE90804732DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="5" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
   </bookViews>
   <sheets>
     <sheet name="Exam A" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Exam B" sheetId="3" r:id="rId3"/>
     <sheet name="Exam C" sheetId="4" r:id="rId4"/>
     <sheet name="Exam A 2" sheetId="5" r:id="rId5"/>
+    <sheet name="Exam B 2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="121">
   <si>
     <t>B</t>
   </si>
@@ -370,6 +371,39 @@
   </si>
   <si>
     <t>89/90</t>
+  </si>
+  <si>
+    <t>2 No Yes No</t>
+  </si>
+  <si>
+    <t>2 Yes No No</t>
+  </si>
+  <si>
+    <t>Remote wipe</t>
+  </si>
+  <si>
+    <t>Host-based firewall</t>
+  </si>
+  <si>
+    <t>Anti-malware</t>
+  </si>
+  <si>
+    <t>Event logs</t>
+  </si>
+  <si>
+    <t>Certificate authority</t>
+  </si>
+  <si>
+    <t>Perfect forward secrecy</t>
+  </si>
+  <si>
+    <t>Data in transit</t>
+  </si>
+  <si>
+    <t>Data at rest</t>
+  </si>
+  <si>
+    <t>Data in use</t>
   </si>
 </sst>
 </file>
@@ -4587,7 +4621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4841A40-96C6-4B3A-A578-4832E7D72006}">
   <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
@@ -5707,4 +5741,544 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89F3912-3C38-4C14-8396-20AD49888B03}">
+  <dimension ref="A1:N90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" t="s">
+        <v>116</v>
+      </c>
+      <c r="N5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" t="s">
+        <v>117</v>
+      </c>
+      <c r="N6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
exam b attempt 2 answers
</commit_message>
<xml_diff>
--- a/ProfessorMesser/PracticeExams.xlsx
+++ b/ProfessorMesser/PracticeExams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\ProfessorMesser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2734900E-9F87-4DA0-8DC6-DE90804732DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2881DC-44E4-46DE-8D05-FCFA3B2F774A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="5" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="123">
   <si>
     <t>B</t>
   </si>
@@ -404,6 +404,12 @@
   </si>
   <si>
     <t>Data in use</t>
+  </si>
+  <si>
+    <t>82/85</t>
+  </si>
+  <si>
+    <t>85/90</t>
   </si>
 </sst>
 </file>
@@ -2341,7 +2347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EADB6D1-012F-48CD-BDB4-09047F70FE9F}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -5748,7 +5754,7 @@
   <dimension ref="A1:N90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5836,6 +5842,13 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF(A6=B6, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
       <c r="F6" t="s">
         <v>101</v>
       </c>
@@ -5850,6 +5863,13 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ref="C7:C70" si="0">IF(A7=B7, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
       <c r="N7" t="s">
         <v>120</v>
       </c>
@@ -5858,6 +5878,13 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
       <c r="N8" t="s">
         <v>120</v>
       </c>
@@ -5866,6 +5893,13 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
       <c r="N9" t="s">
         <v>119</v>
       </c>
@@ -5874,6 +5908,16 @@
       <c r="A10" t="s">
         <v>5</v>
       </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+      <c r="E10" t="s">
+        <v>121</v>
+      </c>
       <c r="N10" t="s">
         <v>119</v>
       </c>
@@ -5882,400 +5926,963 @@
       <c r="A11" t="s">
         <v>4</v>
       </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+      <c r="E11" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" ref="C71:C90" si="1">IF(A71=B71, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>4</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exam c attempt 2 answers
</commit_message>
<xml_diff>
--- a/ProfessorMesser/PracticeExams.xlsx
+++ b/ProfessorMesser/PracticeExams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\ProfessorMesser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2881DC-44E4-46DE-8D05-FCFA3B2F774A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59C3ABF-3AC7-4D22-B5B9-FFB0569CF52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="5" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="3" activeTab="6" xr2:uid="{1795D088-0DDA-4590-B9F8-3E20C0B3889B}"/>
   </bookViews>
   <sheets>
     <sheet name="Exam A" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Exam C" sheetId="4" r:id="rId4"/>
     <sheet name="Exam A 2" sheetId="5" r:id="rId5"/>
     <sheet name="Exam B 2" sheetId="6" r:id="rId6"/>
+    <sheet name="Exam C 2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="127">
   <si>
     <t>B</t>
   </si>
@@ -410,6 +411,18 @@
   </si>
   <si>
     <t>85/90</t>
+  </si>
+  <si>
+    <t>ALLOWED</t>
+  </si>
+  <si>
+    <t>BLOCKED</t>
+  </si>
+  <si>
+    <t>85/85</t>
+  </si>
+  <si>
+    <t>90/90</t>
   </si>
 </sst>
 </file>
@@ -3492,8 +3505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317E6091-B1A7-4EC6-BBEF-8976F22357A5}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="O57" sqref="O57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5753,8 +5766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89F3912-3C38-4C14-8396-20AD49888B03}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6888,4 +6901,1139 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFECED8-7D5B-4F48-A528-21CA9A6B2A0B}">
+  <dimension ref="A1:K90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF(A6=B6, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ref="C7:C70" si="0">IF(A7=B7, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+      <c r="E11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+      <c r="E12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" ref="C71:C90" si="1">IF(A71=B71, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>39</v>
+      </c>
+      <c r="B81" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>